<commit_message>
MultiSheet match report formation done.
</commit_message>
<xml_diff>
--- a/media/testSet1/mergedFile.xlsx
+++ b/media/testSet1/mergedFile.xlsx
@@ -7,14 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Data" sheetId="1" r:id="rId1"/>
+    <sheet name="My Side" sheetId="2" r:id="rId2"/>
+    <sheet name="GST portal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="709">
   <si>
     <t>Particulars</t>
   </si>
@@ -19360,4 +19362,2886 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2">
+        <v>13325.66</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1199.3</v>
+      </c>
+      <c r="H2">
+        <v>1199.3</v>
+      </c>
+      <c r="I2">
+        <v>2398.6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>429</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3">
+        <v>7499</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>674.91</v>
+      </c>
+      <c r="H3">
+        <v>674.91</v>
+      </c>
+      <c r="I3">
+        <v>1349.82</v>
+      </c>
+      <c r="J3" t="s">
+        <v>433</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4">
+        <v>2352.66</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>211.74</v>
+      </c>
+      <c r="H4">
+        <v>211.74</v>
+      </c>
+      <c r="I4">
+        <v>423.48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5">
+        <v>6409.98</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>576.9</v>
+      </c>
+      <c r="H5">
+        <v>576.9</v>
+      </c>
+      <c r="I5">
+        <v>1153.8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>438</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6">
+        <v>8483.5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>763.51</v>
+      </c>
+      <c r="H6">
+        <v>763.51</v>
+      </c>
+      <c r="I6">
+        <v>1527.02</v>
+      </c>
+      <c r="J6" t="s">
+        <v>440</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>15000</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1350</v>
+      </c>
+      <c r="H7">
+        <v>1350</v>
+      </c>
+      <c r="I7">
+        <v>2700</v>
+      </c>
+      <c r="J7" t="s">
+        <v>442</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8">
+        <v>10067</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>906.03</v>
+      </c>
+      <c r="H8">
+        <v>906.03</v>
+      </c>
+      <c r="I8">
+        <v>1812.06</v>
+      </c>
+      <c r="J8" t="s">
+        <v>443</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E9">
+        <v>2030</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>182.7</v>
+      </c>
+      <c r="H9">
+        <v>182.7</v>
+      </c>
+      <c r="I9">
+        <v>365.4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>447</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E10">
+        <v>10408.5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>936.76</v>
+      </c>
+      <c r="H10">
+        <v>936.76</v>
+      </c>
+      <c r="I10">
+        <v>1873.52</v>
+      </c>
+      <c r="J10" t="s">
+        <v>449</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11">
+        <v>8638</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>777.42</v>
+      </c>
+      <c r="H11">
+        <v>777.42</v>
+      </c>
+      <c r="I11">
+        <v>1554.84</v>
+      </c>
+      <c r="J11" t="s">
+        <v>453</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12">
+        <v>18380</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1654.2</v>
+      </c>
+      <c r="H12">
+        <v>1654.2</v>
+      </c>
+      <c r="I12">
+        <v>3308.4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>454</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13">
+        <v>9873</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>888.5700000000001</v>
+      </c>
+      <c r="H13">
+        <v>888.5700000000001</v>
+      </c>
+      <c r="I13">
+        <v>1777.14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>470</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14">
+        <v>8008</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>720.72</v>
+      </c>
+      <c r="H14">
+        <v>720.72</v>
+      </c>
+      <c r="I14">
+        <v>1441.44</v>
+      </c>
+      <c r="J14" t="s">
+        <v>472</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15">
+        <v>5916.83</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>532.51</v>
+      </c>
+      <c r="H15">
+        <v>532.51</v>
+      </c>
+      <c r="I15">
+        <v>1065.02</v>
+      </c>
+      <c r="J15" t="s">
+        <v>476</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16">
+        <v>13517.5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1216.57</v>
+      </c>
+      <c r="H16">
+        <v>1216.57</v>
+      </c>
+      <c r="I16">
+        <v>2433.14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>489</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>288</v>
+      </c>
+      <c r="E17">
+        <v>10049.33</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>904.4299999999999</v>
+      </c>
+      <c r="H17">
+        <v>904.4299999999999</v>
+      </c>
+      <c r="I17">
+        <v>1808.86</v>
+      </c>
+      <c r="J17" t="s">
+        <v>499</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18">
+        <v>12924.16</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1163.17</v>
+      </c>
+      <c r="H18">
+        <v>1163.17</v>
+      </c>
+      <c r="I18">
+        <v>2326.34</v>
+      </c>
+      <c r="J18" t="s">
+        <v>442</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19">
+        <v>4723.23</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>425.1</v>
+      </c>
+      <c r="H19">
+        <v>425.1</v>
+      </c>
+      <c r="I19">
+        <v>850.2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>446</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" t="s">
+        <v>308</v>
+      </c>
+      <c r="E20">
+        <v>1770</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>159.3</v>
+      </c>
+      <c r="H20">
+        <v>159.3</v>
+      </c>
+      <c r="I20">
+        <v>318.6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>516</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" t="s">
+        <v>311</v>
+      </c>
+      <c r="E21">
+        <v>1798</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>161.82</v>
+      </c>
+      <c r="H21">
+        <v>161.82</v>
+      </c>
+      <c r="I21">
+        <v>323.64</v>
+      </c>
+      <c r="J21" t="s">
+        <v>518</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>320</v>
+      </c>
+      <c r="E22">
+        <v>24170</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>2175.3</v>
+      </c>
+      <c r="H22">
+        <v>2175.3</v>
+      </c>
+      <c r="I22">
+        <v>4350.6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>527</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E23">
+        <v>360</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>32.4</v>
+      </c>
+      <c r="H23">
+        <v>32.4</v>
+      </c>
+      <c r="I23">
+        <v>64.8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>508</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
+        <v>325</v>
+      </c>
+      <c r="E24">
+        <v>13895</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1250.55</v>
+      </c>
+      <c r="H24">
+        <v>1250.55</v>
+      </c>
+      <c r="I24">
+        <v>2501.1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>325</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
+        <v>326</v>
+      </c>
+      <c r="E25">
+        <v>675</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>60.75</v>
+      </c>
+      <c r="H25">
+        <v>60.75</v>
+      </c>
+      <c r="I25">
+        <v>121.5</v>
+      </c>
+      <c r="J25" t="s">
+        <v>531</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>327</v>
+      </c>
+      <c r="E26">
+        <v>8100</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>729</v>
+      </c>
+      <c r="H26">
+        <v>729</v>
+      </c>
+      <c r="I26">
+        <v>1458</v>
+      </c>
+      <c r="J26" t="s">
+        <v>532</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>12500</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1125</v>
+      </c>
+      <c r="H27">
+        <v>1125</v>
+      </c>
+      <c r="I27">
+        <v>2250</v>
+      </c>
+      <c r="J27" t="s">
+        <v>534</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>257</v>
+      </c>
+      <c r="E28">
+        <v>7666</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>689.9400000000001</v>
+      </c>
+      <c r="H28">
+        <v>689.9400000000001</v>
+      </c>
+      <c r="I28">
+        <v>1379.88</v>
+      </c>
+      <c r="J28" t="s">
+        <v>474</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E29">
+        <v>11322</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1018.98</v>
+      </c>
+      <c r="H29">
+        <v>1018.98</v>
+      </c>
+      <c r="I29">
+        <v>2037.96</v>
+      </c>
+      <c r="J29" t="s">
+        <v>548</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>374</v>
+      </c>
+      <c r="E30">
+        <v>8059.99</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>725.39</v>
+      </c>
+      <c r="H30">
+        <v>725.39</v>
+      </c>
+      <c r="I30">
+        <v>1450.78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>558</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" t="s">
+        <v>388</v>
+      </c>
+      <c r="E31">
+        <v>12811.36</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1153.02</v>
+      </c>
+      <c r="H31">
+        <v>1153.02</v>
+      </c>
+      <c r="I31">
+        <v>2306.04</v>
+      </c>
+      <c r="J31" t="s">
+        <v>203</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>390</v>
+      </c>
+      <c r="E32">
+        <v>10515.5</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>946.39</v>
+      </c>
+      <c r="H32">
+        <v>946.39</v>
+      </c>
+      <c r="I32">
+        <v>1892.78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>390</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" t="s">
+        <v>394</v>
+      </c>
+      <c r="E33">
+        <v>12720</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1144.8</v>
+      </c>
+      <c r="H33">
+        <v>1144.8</v>
+      </c>
+      <c r="I33">
+        <v>2289.6</v>
+      </c>
+      <c r="J33" t="s">
+        <v>565</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>395</v>
+      </c>
+      <c r="E34">
+        <v>9456.66</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>851.09</v>
+      </c>
+      <c r="H34">
+        <v>851.09</v>
+      </c>
+      <c r="I34">
+        <v>1702.18</v>
+      </c>
+      <c r="J34" t="s">
+        <v>566</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
+        <v>405</v>
+      </c>
+      <c r="E35">
+        <v>11500</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1035</v>
+      </c>
+      <c r="H35">
+        <v>1035</v>
+      </c>
+      <c r="I35">
+        <v>2070</v>
+      </c>
+      <c r="J35" t="s">
+        <v>570</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>412</v>
+      </c>
+      <c r="E36">
+        <v>4084</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>367.56</v>
+      </c>
+      <c r="H36">
+        <v>367.56</v>
+      </c>
+      <c r="I36">
+        <v>735.12</v>
+      </c>
+      <c r="J36" t="s">
+        <v>412</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>3960774.77</v>
+      </c>
+      <c r="F37">
+        <v>40538.75</v>
+      </c>
+      <c r="G37">
+        <v>336202.26</v>
+      </c>
+      <c r="H37">
+        <v>336203.26</v>
+      </c>
+      <c r="I37">
+        <v>712944.27</v>
+      </c>
+      <c r="J37" t="s">
+        <v>534</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>3960774.77</v>
+      </c>
+      <c r="F38">
+        <v>40538.75</v>
+      </c>
+      <c r="G38">
+        <v>336202.26</v>
+      </c>
+      <c r="H38">
+        <v>336203.26</v>
+      </c>
+      <c r="I38">
+        <v>712944.27</v>
+      </c>
+      <c r="J38" t="s">
+        <v>534</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>423</v>
+      </c>
+      <c r="E39">
+        <v>3960774.770000001</v>
+      </c>
+      <c r="F39">
+        <v>40538.75</v>
+      </c>
+      <c r="G39">
+        <v>336202.26</v>
+      </c>
+      <c r="H39">
+        <v>336203.26</v>
+      </c>
+      <c r="I39">
+        <v>712944.2699999999</v>
+      </c>
+      <c r="J39" t="s">
+        <v>423</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>574</v>
+      </c>
+      <c r="K2" t="s">
+        <v>625</v>
+      </c>
+      <c r="L2" t="s">
+        <v>698</v>
+      </c>
+      <c r="M2">
+        <v>2776</v>
+      </c>
+      <c r="N2">
+        <v>2352.66</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>211.74</v>
+      </c>
+      <c r="Q2">
+        <v>211.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>575</v>
+      </c>
+      <c r="K3" t="s">
+        <v>625</v>
+      </c>
+      <c r="L3" t="s">
+        <v>699</v>
+      </c>
+      <c r="M3">
+        <v>7564</v>
+      </c>
+      <c r="N3">
+        <v>6409.98</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>576.9</v>
+      </c>
+      <c r="Q3">
+        <v>576.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>576</v>
+      </c>
+      <c r="K4" t="s">
+        <v>632</v>
+      </c>
+      <c r="L4" t="s">
+        <v>700</v>
+      </c>
+      <c r="M4">
+        <v>5573</v>
+      </c>
+      <c r="N4">
+        <v>4723.23</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>425.1</v>
+      </c>
+      <c r="Q4">
+        <v>425.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>577</v>
+      </c>
+      <c r="K5" t="s">
+        <v>633</v>
+      </c>
+      <c r="L5" t="s">
+        <v>701</v>
+      </c>
+      <c r="M5">
+        <v>2089</v>
+      </c>
+      <c r="N5">
+        <v>1770</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>159.3</v>
+      </c>
+      <c r="Q5">
+        <v>159.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>578</v>
+      </c>
+      <c r="K6" t="s">
+        <v>634</v>
+      </c>
+      <c r="L6" t="s">
+        <v>702</v>
+      </c>
+      <c r="M6">
+        <v>425</v>
+      </c>
+      <c r="N6">
+        <v>360</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>32.4</v>
+      </c>
+      <c r="Q6">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" t="s">
+        <v>635</v>
+      </c>
+      <c r="L7" t="s">
+        <v>703</v>
+      </c>
+      <c r="M7">
+        <v>14750</v>
+      </c>
+      <c r="N7">
+        <v>12500</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1125</v>
+      </c>
+      <c r="Q7">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>579</v>
+      </c>
+      <c r="K8" t="s">
+        <v>595</v>
+      </c>
+      <c r="L8" t="s">
+        <v>704</v>
+      </c>
+      <c r="M8">
+        <v>9449</v>
+      </c>
+      <c r="N8">
+        <v>8008</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>720.72</v>
+      </c>
+      <c r="Q8">
+        <v>720.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>325</v>
+      </c>
+      <c r="K9" t="s">
+        <v>636</v>
+      </c>
+      <c r="L9" t="s">
+        <v>325</v>
+      </c>
+      <c r="M9">
+        <v>16396</v>
+      </c>
+      <c r="N9">
+        <v>13895</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1250.55</v>
+      </c>
+      <c r="Q9">
+        <v>1250.55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>548</v>
+      </c>
+      <c r="K10" t="s">
+        <v>636</v>
+      </c>
+      <c r="L10" t="s">
+        <v>548</v>
+      </c>
+      <c r="M10">
+        <v>13360</v>
+      </c>
+      <c r="N10">
+        <v>11322</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1018.98</v>
+      </c>
+      <c r="Q10">
+        <v>1018.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>565</v>
+      </c>
+      <c r="K11" t="s">
+        <v>636</v>
+      </c>
+      <c r="L11" t="s">
+        <v>565</v>
+      </c>
+      <c r="M11">
+        <v>15010</v>
+      </c>
+      <c r="N11">
+        <v>12720</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1144.8</v>
+      </c>
+      <c r="Q11">
+        <v>1144.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>570</v>
+      </c>
+      <c r="K12" t="s">
+        <v>636</v>
+      </c>
+      <c r="L12" t="s">
+        <v>570</v>
+      </c>
+      <c r="M12">
+        <v>13570</v>
+      </c>
+      <c r="N12">
+        <v>11500</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1035</v>
+      </c>
+      <c r="Q12">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>580</v>
+      </c>
+      <c r="K13" t="s">
+        <v>633</v>
+      </c>
+      <c r="L13" t="s">
+        <v>705</v>
+      </c>
+      <c r="M13">
+        <v>796</v>
+      </c>
+      <c r="N13">
+        <v>675</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>60.75</v>
+      </c>
+      <c r="Q13">
+        <v>60.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>581</v>
+      </c>
+      <c r="K14" t="s">
+        <v>637</v>
+      </c>
+      <c r="L14" t="s">
+        <v>706</v>
+      </c>
+      <c r="M14">
+        <v>2122</v>
+      </c>
+      <c r="N14">
+        <v>1798</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>161.82</v>
+      </c>
+      <c r="Q14">
+        <v>161.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>203</v>
+      </c>
+      <c r="K15" t="s">
+        <v>593</v>
+      </c>
+      <c r="L15" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15">
+        <v>15117</v>
+      </c>
+      <c r="N15">
+        <v>12811.36</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1153.02</v>
+      </c>
+      <c r="Q15">
+        <v>1153.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>